<commit_message>
ElastoDyn: add alias TwrTpTD[xyz]i to the YawBrTD[xyz]i outputs
</commit_message>
<xml_diff>
--- a/docs/OtherSupporting/OutListParameters.xlsx
+++ b/docs/OtherSupporting/OutListParameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aplatt/software-development/GitHub/openfast-bug/docs/OtherSupporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDB8122-8450-AD4C-88E4-CF2C3A1413E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C06F9C-B993-9144-ABB7-5CA4CE177BBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20360" yWindow="-22420" windowWidth="26580" windowHeight="22580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9714" uniqueCount="4928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9717" uniqueCount="4934">
   <si>
     <t>Category</t>
   </si>
@@ -14825,6 +14825,24 @@
   </si>
   <si>
     <t>YawBrTDzi</t>
+  </si>
+  <si>
+    <t>Tower-top / yaw bearing fore-aft (translational) deflection (relative to the undeflected position) including all platform motions</t>
+  </si>
+  <si>
+    <t>Tower-top / yaw bearing side-to-side (translational) deflection (relative to the undeflected position) including all platform motions</t>
+  </si>
+  <si>
+    <t>Tower-top / yaw bearing axial (translational) deflection (relative to the undeflected position) including all platform motions</t>
+  </si>
+  <si>
+    <t>TwrTpTDxi</t>
+  </si>
+  <si>
+    <t>TwrTpTDyi</t>
+  </si>
+  <si>
+    <t>TwrTpTDzi</t>
   </si>
 </sst>
 </file>
@@ -34327,7 +34345,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B332" sqref="B332"/>
+      <selection pane="bottomLeft" activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39838,10 +39856,13 @@
     </row>
     <row r="330" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B330" s="4" t="s">
+        <v>4931</v>
+      </c>
+      <c r="C330" s="4" t="s">
         <v>4925</v>
       </c>
       <c r="D330" s="7" t="s">
-        <v>1000</v>
+        <v>4928</v>
       </c>
       <c r="E330" s="7" t="s">
         <v>691</v>
@@ -39852,10 +39873,13 @@
     </row>
     <row r="331" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B331" s="4" t="s">
+        <v>4932</v>
+      </c>
+      <c r="C331" s="4" t="s">
         <v>4926</v>
       </c>
       <c r="D331" s="7" t="s">
-        <v>1001</v>
+        <v>4929</v>
       </c>
       <c r="E331" s="7" t="s">
         <v>693</v>
@@ -39866,10 +39890,13 @@
     </row>
     <row r="332" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="B332" s="4" t="s">
+        <v>4933</v>
+      </c>
+      <c r="C332" s="4" t="s">
         <v>4927</v>
       </c>
       <c r="D332" s="7" t="s">
-        <v>1002</v>
+        <v>4930</v>
       </c>
       <c r="E332" s="7" t="s">
         <v>695</v>

</xml_diff>